<commit_message>
[#12] minor issues (2)
</commit_message>
<xml_diff>
--- a/results/real_world/fig6_data.xlsx
+++ b/results/real_world/fig6_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kim-yoochan/coding/DeepVM/results/real_world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81673CEC-96C5-914A-B3D2-01729D14EC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24D2204-8E12-1F43-A820-3C37BC1965DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <t>duration</t>
   </si>
   <si>
-    <t>remode_count</t>
+    <t>remote_count</t>
   </si>
 </sst>
 </file>

</xml_diff>